<commit_message>
Finishes integration of QC configuration
</commit_message>
<xml_diff>
--- a/tests/data/GLOS-Climatologies.xlsx
+++ b/tests/data/GLOS-Climatologies.xlsx
@@ -277,7 +277,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -306,9 +306,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1549,314 +1546,324 @@
         <v>-1</v>
       </c>
       <c r="G3" s="9">
-        <v>25</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="K3" s="9">
+        <v>4</v>
+      </c>
+      <c r="L3" s="9">
+        <v>8</v>
+      </c>
       <c r="M3" s="9"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>